<commit_message>
Added Excel of 'listing_sample' table schema
</commit_message>
<xml_diff>
--- a/sql/SmartValuer_MySQLStructure.xlsx
+++ b/sql/SmartValuer_MySQLStructure.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\OneDrive\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\OneDrive\Documents\SmartValuer\sql\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9A106CB2-B36C-4C74-8DC8-25B5C62EF335}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F2BDF2D-605C-4A48-BBCD-2571203B93CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{2ABF527F-9825-42BF-8C31-B5796AADD80F}"/>
   </bookViews>
@@ -33,9 +33,251 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="79">
+  <si>
+    <t>Column Name</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>unit_type</t>
+  </si>
+  <si>
+    <t>Data Type</t>
+  </si>
+  <si>
+    <t>int</t>
+  </si>
+  <si>
+    <t>varchar(255)</t>
+  </si>
+  <si>
+    <t>ENUM('room', 'studio', 'house')</t>
+  </si>
+  <si>
+    <t>NULLABLE</t>
+  </si>
+  <si>
+    <t>Example</t>
+  </si>
+  <si>
+    <t>bedroom_count</t>
+  </si>
+  <si>
+    <t>bathroom_count</t>
+  </si>
+  <si>
+    <t>floor_size_sqft</t>
+  </si>
+  <si>
+    <t>land_size_sqft</t>
+  </si>
+  <si>
+    <t>psf_floor</t>
+  </si>
+  <si>
+    <t>psf_land</t>
+  </si>
+  <si>
+    <t>created_at</t>
+  </si>
+  <si>
+    <t>title</t>
+  </si>
+  <si>
+    <t>address</t>
+  </si>
+  <si>
+    <t>listing_id</t>
+  </si>
+  <si>
+    <t>listing_type</t>
+  </si>
+  <si>
+    <t>ENUM('buy','rent')</t>
+  </si>
+  <si>
+    <t>rent_per_month</t>
+  </si>
+  <si>
+    <t>property_type</t>
+  </si>
+  <si>
+    <t>ENUM('condo','landed','HDB')</t>
+  </si>
+  <si>
+    <t>selling_price</t>
+  </si>
+  <si>
+    <t>ownership_type</t>
+  </si>
+  <si>
+    <t>ENUM('freehold','leasehold')</t>
+  </si>
+  <si>
+    <t>url</t>
+  </si>
+  <si>
+    <t>text</t>
+  </si>
+  <si>
+    <t>property_type_text</t>
+  </si>
+  <si>
+    <t>ownership_type_text</t>
+  </si>
+  <si>
+    <t>selling_price_text</t>
+  </si>
+  <si>
+    <t>rent_per_month_text</t>
+  </si>
+  <si>
+    <t>double</t>
+  </si>
+  <si>
+    <t>timestamp</t>
+  </si>
+  <si>
+    <t>availability</t>
+  </si>
+  <si>
+    <t>"Ready to Move" | "Available from 19 Jun"</t>
+  </si>
+  <si>
+    <t>Remarks</t>
+  </si>
+  <si>
+    <t>Not available for "rent" listing_type</t>
+  </si>
+  <si>
+    <t>project_year</t>
+  </si>
+  <si>
+    <t>Taken from "Built: 2023" or "New Project: 2025"</t>
+  </si>
+  <si>
+    <t>Auto increment</t>
+  </si>
+  <si>
+    <t>"11 Buckley Road"</t>
+  </si>
+  <si>
+    <t>"Buckley Classique"</t>
+  </si>
+  <si>
+    <t>https://www.propertyguru.com.sg/listing/for-rent-buckley-classique-21290969</t>
+  </si>
+  <si>
+    <t>2025-04-15 01:11:16</t>
+  </si>
+  <si>
+    <t>CURRENT_TIMESTAMP</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>Taken from "Listed on Apr 15, 2025 (47m ago)"</t>
+  </si>
+  <si>
+    <t>listed_date</t>
+  </si>
+  <si>
+    <t>2025-04-15</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>distance_to_closest_MRT</t>
+  </si>
+  <si>
+    <t>Taken from text "1.5 km (18 mins) from JE7 Pandan Reservoir MRT"</t>
+  </si>
+  <si>
+    <t>1500</t>
+  </si>
+  <si>
+    <t>"Bungalow House" | "Aparment" | "Condominium" | "HDB Flat" | "Semi-Detached House" | "Detached House" | " Corner Terrace" | "Executive Condominium"</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Available for "buy" listing_type</t>
+  </si>
+  <si>
+    <t>"Freehold" | "99-year leasehold"</t>
+  </si>
+  <si>
+    <t>is_verified_listing</t>
+  </si>
+  <si>
+    <t>boolean</t>
+  </si>
+  <si>
+    <t>"True" | "False"</t>
+  </si>
+  <si>
+    <t>"True" if "Verified Listing" tag exists, else "False"</t>
+  </si>
+  <si>
+    <t>NULL for 'rent'</t>
+  </si>
+  <si>
+    <t>NULL for 'buy'</t>
+  </si>
+  <si>
+    <t>S$ 4,800 /mo</t>
+  </si>
+  <si>
+    <t>4800</t>
+  </si>
+  <si>
+    <t>S$ 10,223,456</t>
+  </si>
+  <si>
+    <t>10,223,456</t>
+  </si>
+  <si>
+    <t>Will have "(land)" after "S$6.00 psf"</t>
+  </si>
+  <si>
+    <t>If does not have "(land)" after "S$6.00 psf", default to floor</t>
+  </si>
+  <si>
+    <t>For 'room', it only shows "Room",  no count. For this, put 0. If no this section, then only null. For 'studio', it only shows "Studio", no count. For this put 0. If no this section, then only null.</t>
+  </si>
+  <si>
+    <t>For all, it sometimes has bathroom count, sometimes no</t>
+  </si>
+  <si>
+    <t>agent_name</t>
+  </si>
+  <si>
+    <t>"Zarin Fathima Riaz"</t>
+  </si>
+  <si>
+    <t>is_everyone_welcomed</t>
+  </si>
+  <si>
+    <t>"True" if "Everyone Welcome" tag exists, else "False"</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>Unique</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -43,16 +285,38 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -60,14 +324,184 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="8" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -380,14 +814,522 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{171B914C-1C7A-48C3-9349-5216D8861CA8}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16" defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="34.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="38.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="16" style="1"/>
+    <col min="4" max="4" width="54" style="1" customWidth="1"/>
+    <col min="5" max="5" width="75.5703125" style="2" customWidth="1"/>
+    <col min="6" max="16384" width="16" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="9">
+        <v>0</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="4">
+        <v>0</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="E3" s="12">
+        <v>25529453</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="4">
+        <v>0</v>
+      </c>
+      <c r="D4" s="4"/>
+      <c r="E4" s="12" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="4">
+        <v>0</v>
+      </c>
+      <c r="D5" s="4"/>
+      <c r="E5" s="12" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" s="4">
+        <v>0</v>
+      </c>
+      <c r="D6" s="4"/>
+      <c r="E6" s="13" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" s="4">
+        <v>1</v>
+      </c>
+      <c r="D7" s="4"/>
+      <c r="E7" s="14" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="4">
+        <v>1</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="E8" s="14">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="4">
+        <v>1</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="E9" s="14" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" s="4">
+        <v>1</v>
+      </c>
+      <c r="D10" s="4"/>
+      <c r="E10" s="14"/>
+    </row>
+    <row r="11" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C11" s="4">
+        <v>1</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="E11" s="14" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C12" s="4">
+        <v>1</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="E12" s="14" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C13" s="4">
+        <v>0</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="E13" s="14" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14" s="4">
+        <v>0</v>
+      </c>
+      <c r="D14" s="4"/>
+      <c r="E14" s="14" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C15" s="4">
+        <v>0</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="E15" s="12" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C16" s="9">
+        <v>0</v>
+      </c>
+      <c r="D16" s="9"/>
+      <c r="E16" s="15" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="B17" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="C17" s="17">
+        <v>1</v>
+      </c>
+      <c r="D17" s="17"/>
+      <c r="E17" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B18" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C18" s="9">
+        <v>1</v>
+      </c>
+      <c r="D18" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="E18" s="10" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="B19" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="C19" s="17">
+        <v>1</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B20" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C20" s="9">
+        <v>0</v>
+      </c>
+      <c r="D20" s="9"/>
+      <c r="E20" s="10" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C21" s="4">
+        <v>1</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="E21" s="12" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C22" s="4">
+        <v>1</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="E22" s="12" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C23" s="4">
+        <v>1</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="E23" s="12" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="B24" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="C24" s="17">
+        <v>1</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="B25" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C25" s="9">
+        <v>0</v>
+      </c>
+      <c r="D25" s="9"/>
+      <c r="E25" s="10" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C26" s="4">
+        <v>1</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="E26" s="12"/>
+    </row>
+    <row r="27" spans="1:5" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C27" s="4">
+        <v>1</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="E27" s="12"/>
+    </row>
+    <row r="28" spans="1:5" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C28" s="4">
+        <v>1</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="E28" s="12"/>
+    </row>
+    <row r="29" spans="1:5" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C29" s="4">
+        <v>1</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="E29" s="12"/>
+    </row>
+    <row r="30" spans="1:5" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C30" s="4">
+        <v>1</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="E30" s="12"/>
+    </row>
+    <row r="31" spans="1:5" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="B31" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="C31" s="17">
+        <v>1</v>
+      </c>
+      <c r="D31" s="17" t="s">
+        <v>69</v>
+      </c>
+      <c r="E31" s="3"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E6" r:id="rId1" xr:uid="{F3BCA091-CC05-48F7-B101-D9D4D1834B4B}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError sqref="E23 E21" numberStoredAsText="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>